<commit_message>
Split patient / HP tests
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-cthp.xlsx
+++ b/test-data/webanalytics-cthp.xlsx
@@ -8,17 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E7360808-470C-4DC3-9862-6D506CD8207B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BFE03EA2-59CA-473C-B857-40B1EC02AD04}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CTHPPage" sheetId="5" r:id="rId1"/>
-    <sheet name="ErrorPage" sheetId="10" r:id="rId2"/>
-    <sheet name="HomePage" sheetId="2" r:id="rId3"/>
-    <sheet name="InnerPage" sheetId="1" r:id="rId4"/>
-    <sheet name="LandingPage" sheetId="3" r:id="rId5"/>
-    <sheet name="TopicPage" sheetId="4" r:id="rId6"/>
+    <sheet name="CTHPHPCard" sheetId="10" r:id="rId2"/>
+    <sheet name="CTHPPatientCard" sheetId="12" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -30,77 +27,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
   <si>
     <t>Path</t>
   </si>
   <si>
-    <t>/about-nci/visit</t>
-  </si>
-  <si>
     <t>ContentType</t>
   </si>
   <si>
-    <t>Article</t>
-  </si>
-  <si>
-    <t>General</t>
-  </si>
-  <si>
-    <t>/about-nci/overview</t>
-  </si>
-  <si>
-    <t>/espanol/instituto/general</t>
-  </si>
-  <si>
-    <t>/espanol/acerca-sitio/mapa-sitio</t>
-  </si>
-  <si>
-    <t>/</t>
-  </si>
-  <si>
-    <t>Site Home</t>
-  </si>
-  <si>
-    <t>Landing Page</t>
-  </si>
-  <si>
-    <t>/about-nci</t>
-  </si>
-  <si>
-    <t>/espanol/instituto</t>
-  </si>
-  <si>
-    <t>/news-events</t>
-  </si>
-  <si>
-    <t>/espanol/noticias</t>
-  </si>
-  <si>
-    <t>/espanol</t>
-  </si>
-  <si>
-    <t>/sites/nano</t>
-  </si>
-  <si>
-    <t>Home/Landing Page</t>
-  </si>
-  <si>
-    <t>/about-cancer/treatment</t>
-  </si>
-  <si>
-    <t>/espanol/cancer/tratamiento</t>
-  </si>
-  <si>
-    <t>/resources-for</t>
-  </si>
-  <si>
-    <t>/espanol/recursos-para</t>
-  </si>
-  <si>
-    <t>Topic Page</t>
-  </si>
-  <si>
     <t>CTHP HP</t>
   </si>
   <si>
@@ -119,22 +53,58 @@
     <t>/types/lung/hp</t>
   </si>
   <si>
-    <t>Error Page</t>
-  </si>
-  <si>
-    <t>Thank You</t>
-  </si>
-  <si>
-    <t>Page Not Found</t>
-  </si>
-  <si>
-    <t>/PublishedContent/ErrorMessages/Error.html</t>
-  </si>
-  <si>
-    <t>/PublishedContent/ErrorMessages/ThankYou.html</t>
-  </si>
-  <si>
-    <t>/PublishedContent/ErrorMessages/PageNotFound.html</t>
+    <t>/types/bladder</t>
+  </si>
+  <si>
+    <t>/types/breast/hp</t>
+  </si>
+  <si>
+    <t>Audience</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>CardTitle</t>
+  </si>
+  <si>
+    <t>LinkText</t>
+  </si>
+  <si>
+    <t>Overview</t>
+  </si>
+  <si>
+    <t>Bladder Cancer Symptoms, Tests, Prognosis, and Stages</t>
+  </si>
+  <si>
+    <t>CTHP:1</t>
+  </si>
+  <si>
+    <t>CardPos</t>
+  </si>
+  <si>
+    <t>Bladder and Other Urothelial Cancers Screening</t>
+  </si>
+  <si>
+    <t>Screening</t>
+  </si>
+  <si>
+    <t>CTHP:4</t>
+  </si>
+  <si>
+    <t>Treatment</t>
+  </si>
+  <si>
+    <t>Supportive &amp; Palliative Care</t>
+  </si>
+  <si>
+    <t>Nausea and Vomiting</t>
+  </si>
+  <si>
+    <t>CTHP:6</t>
+  </si>
+  <si>
+    <t>Male Breast Cancer Treatment</t>
   </si>
 </sst>
 </file>
@@ -184,9 +154,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,54 +475,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -560,48 +532,70 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F2B56E1-BA35-4071-8CAC-1CCCC51E0A7D}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" t="s">
-        <v>30</v>
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -611,231 +605,65 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EE3E006-14B8-4210-9A28-7DC7E1128698}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" t="s">
-        <v>17</v>
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="30.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.54296875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="27.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Spanish data for CTHP cards
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-cthp.xlsx
+++ b/test-data/webanalytics-cthp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BFE03EA2-59CA-473C-B857-40B1EC02AD04}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{DABA66F5-23A8-48F0-8EED-7FB28C1AC82B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CTHPPage" sheetId="5" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
   <si>
     <t>Path</t>
   </si>
@@ -105,6 +105,39 @@
   </si>
   <si>
     <t>Male Breast Cancer Treatment</t>
+  </si>
+  <si>
+    <t>CTHP:2</t>
+  </si>
+  <si>
+    <t>Leucemia de células pilosas</t>
+  </si>
+  <si>
+    <t>Tratamiento</t>
+  </si>
+  <si>
+    <t>/espanol/tipos/leucemia</t>
+  </si>
+  <si>
+    <t>Aspectos generales de la prevención del cáncer (PDQ®)</t>
+  </si>
+  <si>
+    <t>Causas y prevención</t>
+  </si>
+  <si>
+    <t>CTHP:3</t>
+  </si>
+  <si>
+    <t>/espanol/tipos/cabeza-cuello</t>
+  </si>
+  <si>
+    <t>Detección del cáncer de cavidad oral, faringe y laringe</t>
+  </si>
+  <si>
+    <t>CTHP:5</t>
+  </si>
+  <si>
+    <t>Exámenes de detección</t>
   </si>
 </sst>
 </file>
@@ -532,18 +565,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F2B56E1-BA35-4071-8CAC-1CCCC51E0A7D}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="3"/>
   </cols>
   <sheetData>
@@ -596,6 +629,23 @@
       </c>
       <c r="E3" s="3" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -606,16 +656,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EE3E006-14B8-4210-9A28-7DC7E1128698}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="51" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
@@ -662,6 +712,34 @@
         <v>20</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>